<commit_message>
#11 change some weapon data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassic\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Job" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="101">
   <si>
     <t>arrow</t>
   </si>
@@ -221,38 +221,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>可以给己方单位装备一把铁锤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以给己方单位装备一面铁盾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对目标造成长时间的流血状态</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对一个单体目标造成魔法伤害，对英雄造成双倍伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>一定概率抽一张牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对一个单体目标造成魔法伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>回复一个己方单位生命值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>消耗魔法值来获取一定的怒气值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>所有怪物等级+1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -345,10 +313,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>蠢事装备</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>21400101</t>
   </si>
   <si>
@@ -369,6 +333,102 @@
   </si>
   <si>
     <t>11000000|NewBie</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>水</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>风</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>光</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲锋战</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击战</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复盾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>刺杀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>下毒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>输出</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰法</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火法</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奶</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑暗贤者</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝福</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>光环怪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>武器强化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>远程强化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>伤害强化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始装备</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1013,7 +1073,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1036,6 +1096,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1117,7 +1183,7 @@
     <tableColumn id="35" name="魔法点获取的比率"/>
     <tableColumn id="4" name="初始的额外卡牌"/>
     <tableColumn id="6" name="初始道具" dataDxfId="1"/>
-    <tableColumn id="7" name="蠢事装备" dataDxfId="0"/>
+    <tableColumn id="7" name="初始装备" dataDxfId="0"/>
     <tableColumn id="12" name="形象"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1414,19 +1480,19 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.875" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="4" max="4" width="42.625" customWidth="1"/>
-    <col min="5" max="5" width="10.125" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1443,19 +1509,19 @@
         <v>29</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1472,19 +1538,19 @@
         <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1501,21 +1567,21 @@
         <v>44</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -1530,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11000001</v>
       </c>
@@ -1547,19 +1613,19 @@
         <v>31</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>11000002</v>
       </c>
@@ -1576,17 +1642,17 @@
         <v>31</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11000003</v>
       </c>
@@ -1603,7 +1669,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -1611,7 +1677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11000004</v>
       </c>
@@ -1630,13 +1696,13 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="I8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11000005</v>
       </c>
@@ -1659,7 +1725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11000006</v>
       </c>
@@ -1682,7 +1748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11000007</v>
       </c>
@@ -1705,7 +1771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11000008</v>
       </c>
@@ -1741,19 +1807,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="4" width="35" customWidth="1"/>
+    <col min="5" max="11" width="7.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -1766,8 +1833,29 @@
       <c r="D1" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
@@ -1775,124 +1863,148 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="G3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="I4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+        <v>49</v>
+      </c>
+      <c r="J9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="6" t="s">
-        <v>55</v>
+      <c r="E10" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some weapon card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Job" sheetId="1" r:id="rId1"/>
@@ -1480,19 +1480,19 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="42.625" customWidth="1"/>
+    <col min="5" max="5" width="10.125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>11000001</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>11000002</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>11000003</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>11000004</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>11000005</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>11000006</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>11000007</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11000008</v>
       </c>
@@ -1813,14 +1813,14 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="4" width="35" customWidth="1"/>
-    <col min="5" max="11" width="7.77734375" customWidth="1"/>
+    <col min="5" max="11" width="7.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
@@ -1863,7 +1863,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
job differ point limit #29
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Job" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,37 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>real</author>
     <author>张剑慧</author>
   </authors>
   <commentList>
     <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>real:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Lp:Pp:Mp</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="118">
   <si>
     <t>arrow</t>
   </si>
@@ -197,251 +224,303 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>InitialCards</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始的额外卡牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>InitialItem</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>InitialEquip</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>21400101</t>
+  </si>
+  <si>
+    <t>22032007</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>53000001</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>53000002</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>53000003,53000004</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>11000000|NewBie</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>水</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>风</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>光</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲锋战</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击战</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复盾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>刺杀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>下毒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>输出</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰法</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火法</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奶</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝福</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>光环怪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>武器强化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>远程强化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>伤害强化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始装备</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>JobIndex</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>颜色</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Color</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yellow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pink</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brown</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Purple</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Green</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死灵</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkfire</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gray</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在所有的黑魔法中最为黑暗的毫无疑问的非死灵术/通幽术（Necromancy）莫属！而且也是最丑恶和最令人厌恶的魔法仪式之一。而死灵术本身是指古代与死亡世界沟通的一种方法。死灵魔法可以追述到古波斯、希腊、罗马和中世纪的巫师。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>猎人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Salmon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>萨满</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aqua</t>
+  </si>
+  <si>
+    <t>electball</t>
+  </si>
+  <si>
+    <t>萨满祭司是自己部落和氏族的精神领袖。他们是操纵元素的大师，既能引导能量摧毁敌人，也能汇聚法力增强队友。在各种图腾的帮助下，萨满能凝聚不羁元素的能量，化身为全能的战士。</t>
+  </si>
+  <si>
+    <t>萨满</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷系</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>法术</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnergyLimit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>能量值上限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>EnergyRate</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>int[]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>InitialCards</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始的额外卡牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int[]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>InitialItem</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>InitialEquip</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>21400101</t>
-  </si>
-  <si>
-    <t>22032007</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>53000001</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>53000002</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>53000003,53000004</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>11000000|NewBie</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>水</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>风</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>火</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>地</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>光</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>暗</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冲锋战</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击战</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>回复盾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>刺杀</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>下毒</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>输出</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冰法</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>火法</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>奶</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>祝福</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>光环怪</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>武器强化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>远程强化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>伤害强化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始装备</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>JobIndex</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>颜色</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Color</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yellow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pink</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brown</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Purple</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Green</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死灵</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkfire</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gray</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>在所有的黑魔法中最为黑暗的毫无疑问的非死灵术/通幽术（Necromancy）莫属！而且也是最丑恶和最令人厌恶的魔法仪式之一。而死灵术本身是指古代与死亡世界沟通的一种方法。死灵魔法可以追述到古波斯、希腊、罗马和中世纪的巫师。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>猎人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Salmon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Blue</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>萨满</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Aqua</t>
-  </si>
-  <si>
-    <t>electball</t>
-  </si>
-  <si>
-    <t>萨满祭司是自己部落和氏族的精神领袖。他们是操纵元素的大师，既能引导能量摧毁敌人，也能汇聚法力增强队友。在各种图腾的帮助下，萨满能凝聚不羁元素的能量，化身为全能的战士。</t>
-  </si>
-  <si>
-    <t>萨满</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>雷系</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>法术</t>
+    <t>5;5;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>8;8;6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>7;5;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>6;6;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>8;6;8</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>8;8;7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>7;7;8</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>9;9;4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>8;9;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>9;7;6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>6;10;6</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1186,13 +1265,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:J14" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:J14"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K14" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:K14"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="序列"/>
     <tableColumn id="2" name="名字"/>
     <tableColumn id="19" name="箭矢"/>
     <tableColumn id="33" name="描述"/>
+    <tableColumn id="5" name="能量值上限"/>
     <tableColumn id="35" name="魔法点获取的比率"/>
     <tableColumn id="4" name="初始的额外卡牌"/>
     <tableColumn id="6" name="初始道具" dataDxfId="1"/>
@@ -1491,22 +1571,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="42.625" customWidth="1"/>
+    <col min="5" max="5" width="10.125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1520,25 +1600,28 @@
         <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1555,22 +1638,25 @@
         <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1584,27 +1670,30 @@
         <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -1613,16 +1702,19 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" t="s">
         <v>37</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>11000001</v>
       </c>
@@ -1636,10 +1728,10 @@
         <v>39</v>
       </c>
       <c r="E5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" t="s">
         <v>31</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>51</v>
@@ -1647,14 +1739,17 @@
       <c r="H5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="J5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>11000002</v>
       </c>
@@ -1668,23 +1763,26 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>53</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6">
+        <v>52</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6">
         <v>2</v>
       </c>
-      <c r="J6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>11000003</v>
       </c>
@@ -1698,26 +1796,29 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="H7" s="7"/>
-      <c r="I7">
+      <c r="I7" s="7"/>
+      <c r="J7">
         <v>3</v>
       </c>
-      <c r="J7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>11000004</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -1726,21 +1827,24 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8">
+      <c r="H8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8">
         <v>4</v>
       </c>
-      <c r="J8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>11000005</v>
       </c>
@@ -1754,19 +1858,22 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9">
+      <c r="I9" s="7"/>
+      <c r="J9">
         <v>5</v>
       </c>
-      <c r="J9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>11000006</v>
       </c>
@@ -1780,19 +1887,22 @@
         <v>40</v>
       </c>
       <c r="E10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10">
+      <c r="I10" s="7"/>
+      <c r="J10">
         <v>6</v>
       </c>
-      <c r="J10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>11000007</v>
       </c>
@@ -1806,19 +1916,22 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11">
+      <c r="I11" s="7"/>
+      <c r="J11">
         <v>7</v>
       </c>
-      <c r="J11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11000008</v>
       </c>
@@ -1832,68 +1945,77 @@
         <v>41</v>
       </c>
       <c r="E12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12">
+      <c r="I12" s="7"/>
+      <c r="J12">
         <v>8</v>
       </c>
-      <c r="J12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>11000009</v>
       </c>
       <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
         <v>91</v>
       </c>
-      <c r="C13" t="s">
-        <v>92</v>
-      </c>
       <c r="D13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13">
+      <c r="I13" s="7"/>
+      <c r="J13">
         <v>9</v>
       </c>
-      <c r="J13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11000010</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" t="s">
         <v>100</v>
       </c>
-      <c r="D14" t="s">
-        <v>101</v>
-      </c>
       <c r="E14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14">
+      <c r="I14" s="7"/>
+      <c r="J14">
         <v>10</v>
       </c>
-      <c r="J14" t="s">
-        <v>97</v>
+      <c r="K14" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1911,149 +2033,149 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="8" width="7.77734375" customWidth="1"/>
+    <col min="2" max="8" width="7.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
         <v>63</v>
       </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" t="s">
         <v>65</v>
       </c>
-      <c r="G4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" t="s">
         <v>76</v>
       </c>
-      <c r="E6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" t="s">
         <v>70</v>
       </c>
-      <c r="E8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" t="s">
         <v>102</v>
-      </c>
-      <c r="E12" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
close #43 finish job's given
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Job" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="127">
   <si>
     <t>arrow</t>
   </si>
@@ -541,6 +541,14 @@
   </si>
   <si>
     <t>22032005</t>
+  </si>
+  <si>
+    <t>21200421</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>21300311</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1593,20 +1601,20 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.875" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="4" max="4" width="42.625" customWidth="1"/>
-    <col min="5" max="5" width="10.125" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="22.25" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1641,7 +1649,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1676,7 +1684,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1711,7 +1719,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1734,7 +1742,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11000001</v>
       </c>
@@ -1757,7 +1765,9 @@
         <v>112</v>
       </c>
       <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="J5">
         <v>1</v>
       </c>
@@ -1765,7 +1775,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>11000002</v>
       </c>
@@ -1796,7 +1806,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11000003</v>
       </c>
@@ -1829,7 +1839,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11000004</v>
       </c>
@@ -1852,7 +1862,9 @@
         <v>116</v>
       </c>
       <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="J8">
         <v>4</v>
       </c>
@@ -1860,7 +1872,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11000005</v>
       </c>
@@ -1891,7 +1903,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11000006</v>
       </c>
@@ -1922,7 +1934,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11000007</v>
       </c>
@@ -1953,7 +1965,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11000008</v>
       </c>
@@ -1986,7 +1998,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11000009</v>
       </c>
@@ -2019,7 +2031,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11000010</v>
       </c>
@@ -2069,13 +2081,13 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="8" width="7.75" customWidth="1"/>
+    <col min="2" max="8" width="7.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -2101,12 +2113,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -2117,7 +2129,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -2128,7 +2140,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -2139,7 +2151,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -2150,7 +2162,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -2161,7 +2173,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -2172,7 +2184,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -2183,7 +2195,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -2194,7 +2206,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>85</v>
       </c>
@@ -2202,7 +2214,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
special job for activity role
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Job" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="137">
   <si>
     <t>arrow</t>
   </si>
@@ -252,302 +252,340 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>水</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>风</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>光</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲锋战</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击战</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复盾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>刺杀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>下毒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>输出</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰法</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>火法</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奶</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝福</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>光环怪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>武器强化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>远程强化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>伤害强化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始装备</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>JobIndex</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>颜色</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Color</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yellow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pink</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brown</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Purple</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Green</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死灵</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkfire</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gray</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在所有的黑魔法中最为黑暗的毫无疑问的非死灵术/通幽术（Necromancy）莫属！而且也是最丑恶和最令人厌恶的魔法仪式之一。而死灵术本身是指古代与死亡世界沟通的一种方法。死灵魔法可以追述到古波斯、希腊、罗马和中世纪的巫师。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>猎人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Salmon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>萨满</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aqua</t>
+  </si>
+  <si>
+    <t>electball</t>
+  </si>
+  <si>
+    <t>萨满祭司是自己部落和氏族的精神领袖。他们是操纵元素的大师，既能引导能量摧毁敌人，也能汇聚法力增强队友。在各种图腾的帮助下，萨满能凝聚不羁元素的能量，化身为全能的战士。</t>
+  </si>
+  <si>
+    <t>萨满</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷系</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>法术</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnergyLimit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>能量值上限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnergyRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>5;5;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>9;10;7</t>
+  </si>
+  <si>
+    <t>10;8;8</t>
+  </si>
+  <si>
+    <t>9;9;8</t>
+  </si>
+  <si>
+    <t>10;10;6</t>
+  </si>
+  <si>
+    <t>7;11;8</t>
+  </si>
+  <si>
+    <t>8;7;11</t>
+  </si>
+  <si>
+    <t>10;6;10</t>
+  </si>
+  <si>
+    <t>9;8;9</t>
+  </si>
+  <si>
+    <t>7;9;10</t>
+  </si>
+  <si>
+    <t>52000094</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>52000019,53000109</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>22032008</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>52000104</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>52000023</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>52000065,53000099</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>53000014,53000018</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>53000015,53000060</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>53000085</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>53000043</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>52000038,53000081</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>22032006</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>22032005</t>
+  </si>
+  <si>
+    <t>21200421</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>21300311</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否常规职业</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>isSpecial</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100;0;0</t>
+  </si>
+  <si>
+    <t>10;3;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动2</t>
+  </si>
+  <si>
+    <t>50;20;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>10;10;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>11000000|NewBie</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>水</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>风</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>火</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>地</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>光</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>暗</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冲锋战</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击战</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>回复盾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>刺杀</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>下毒</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>输出</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冰法</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>火法</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>奶</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>祝福</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>光环怪</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>武器强化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>远程强化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>伤害强化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始装备</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>JobIndex</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>颜色</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Color</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yellow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pink</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Black</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brown</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Purple</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Green</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死灵</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkfire</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gray</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>在所有的黑魔法中最为黑暗的毫无疑问的非死灵术/通幽术（Necromancy）莫属！而且也是最丑恶和最令人厌恶的魔法仪式之一。而死灵术本身是指古代与死亡世界沟通的一种方法。死灵魔法可以追述到古波斯、希腊、罗马和中世纪的巫师。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>猎人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Salmon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Blue</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>萨满</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Aqua</t>
-  </si>
-  <si>
-    <t>electball</t>
-  </si>
-  <si>
-    <t>萨满祭司是自己部落和氏族的精神领袖。他们是操纵元素的大师，既能引导能量摧毁敌人，也能汇聚法力增强队友。在各种图腾的帮助下，萨满能凝聚不羁元素的能量，化身为全能的战士。</t>
-  </si>
-  <si>
-    <t>萨满</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>雷系</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>法术</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>EnergyLimit</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>能量值上限</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>EnergyRate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>5;5;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>9;10;7</t>
-  </si>
-  <si>
-    <t>10;8;8</t>
-  </si>
-  <si>
-    <t>9;9;8</t>
-  </si>
-  <si>
-    <t>10;10;6</t>
-  </si>
-  <si>
-    <t>7;11;8</t>
-  </si>
-  <si>
-    <t>8;7;11</t>
-  </si>
-  <si>
-    <t>10;6;10</t>
-  </si>
-  <si>
-    <t>9;8;9</t>
-  </si>
-  <si>
-    <t>7;9;10</t>
-  </si>
-  <si>
-    <t>52000094</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>52000019,53000109</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>22032008</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>52000104</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>52000023</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>52000065,53000099</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>53000014,53000018</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>53000015,53000060</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>53000085</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>53000043</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>52000038,53000081</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>22032006</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>22032005</t>
-  </si>
-  <si>
-    <t>21200421</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>21300311</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1292,9 +1330,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K14" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:K14"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L16" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:L16"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="序列"/>
     <tableColumn id="2" name="名字"/>
     <tableColumn id="19" name="箭矢"/>
@@ -1306,6 +1344,7 @@
     <tableColumn id="7" name="初始装备" dataDxfId="0"/>
     <tableColumn id="12" name="形象"/>
     <tableColumn id="3" name="颜色"/>
+    <tableColumn id="8" name="是否常规职业"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1598,23 +1637,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="42.625" customWidth="1"/>
+    <col min="5" max="5" width="10.125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="22.21875" customWidth="1"/>
+    <col min="7" max="7" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1628,7 +1667,7 @@
         <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>29</v>
@@ -1640,16 +1679,19 @@
         <v>48</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>38</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1678,13 +1720,16 @@
         <v>45</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1698,10 +1743,10 @@
         <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>43</v>
@@ -1713,15 +1758,18 @@
         <v>47</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -1730,7 +1778,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" t="s">
         <v>37</v>
@@ -1739,10 +1787,13 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>11000001</v>
       </c>
@@ -1756,26 +1807,27 @@
         <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" t="s">
         <v>31</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>11000002</v>
       </c>
@@ -1789,13 +1841,13 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
         <v>31</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -1803,10 +1855,11 @@
         <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>11000003</v>
       </c>
@@ -1820,31 +1873,32 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7">
         <v>3</v>
       </c>
       <c r="K7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>11000004</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -1853,26 +1907,27 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" t="s">
         <v>31</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J8">
         <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>11000005</v>
       </c>
@@ -1886,13 +1941,13 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -1900,10 +1955,11 @@
         <v>5</v>
       </c>
       <c r="K9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>11000006</v>
       </c>
@@ -1917,13 +1973,13 @@
         <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1931,10 +1987,11 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>11000007</v>
       </c>
@@ -1948,13 +2005,13 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F11" t="s">
         <v>35</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -1962,10 +2019,11 @@
         <v>7</v>
       </c>
       <c r="K11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11000008</v>
       </c>
@@ -1979,79 +2037,81 @@
         <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F12" t="s">
         <v>36</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12">
         <v>8</v>
       </c>
       <c r="K12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>11000009</v>
       </c>
       <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
         <v>85</v>
       </c>
-      <c r="C13" t="s">
-        <v>86</v>
-      </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F13" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13">
         <v>9</v>
       </c>
       <c r="K13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11000010</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" t="s">
         <v>94</v>
       </c>
-      <c r="D14" t="s">
-        <v>95</v>
-      </c>
       <c r="E14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F14" t="s">
         <v>31</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -2059,7 +2119,66 @@
         <v>10</v>
       </c>
       <c r="K14" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>11001001</v>
+      </c>
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>79</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>11001002</v>
+      </c>
+      <c r="B16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>79</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2081,145 +2200,145 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="8" width="7.77734375" customWidth="1"/>
+    <col min="2" max="8" width="7.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
         <v>57</v>
       </c>
-      <c r="E3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" t="s">
         <v>59</v>
       </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
         <v>70</v>
       </c>
-      <c r="E6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s">
         <v>64</v>
       </c>
-      <c r="E8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" t="s">
         <v>96</v>
-      </c>
-      <c r="E12" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#58 add a card for poet
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Job" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="141">
   <si>
     <t>arrow</t>
   </si>
@@ -598,6 +598,10 @@
   </si>
   <si>
     <t>50;20;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>坟墓</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -791,7 +795,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -974,6 +978,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1242,7 +1252,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1271,6 +1281,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1652,20 +1665,20 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.875" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="4" max="4" width="42.625" customWidth="1"/>
-    <col min="5" max="5" width="10.125" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="22.25" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1703,7 +1716,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1741,7 +1754,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1779,7 +1792,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -1805,7 +1818,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11000001</v>
       </c>
@@ -1839,7 +1852,7 @@
       </c>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>11000002</v>
       </c>
@@ -1871,7 +1884,7 @@
       </c>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11000003</v>
       </c>
@@ -1905,7 +1918,7 @@
       </c>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11000004</v>
       </c>
@@ -1939,7 +1952,7 @@
       </c>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11000005</v>
       </c>
@@ -1971,7 +1984,7 @@
       </c>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11000006</v>
       </c>
@@ -2003,7 +2016,7 @@
       </c>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11000007</v>
       </c>
@@ -2035,7 +2048,7 @@
       </c>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11000008</v>
       </c>
@@ -2069,7 +2082,7 @@
       </c>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11000009</v>
       </c>
@@ -2103,7 +2116,7 @@
       </c>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11000010</v>
       </c>
@@ -2135,7 +2148,7 @@
       </c>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11001001</v>
       </c>
@@ -2164,7 +2177,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11001002</v>
       </c>
@@ -2206,19 +2219,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="8" width="7.75" customWidth="1"/>
+    <col min="2" max="8" width="7.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -2244,12 +2257,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -2260,7 +2273,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -2271,7 +2284,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -2282,7 +2295,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -2293,7 +2306,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -2304,7 +2317,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -2315,7 +2328,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -2326,7 +2339,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -2337,15 +2350,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>77</v>
       </c>
       <c r="H11" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J11" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
fix the card #58
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="141">
   <si>
     <t>arrow</t>
   </si>
@@ -519,10 +519,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>是否常规职业</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>bool</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -602,6 +598,10 @@
   </si>
   <si>
     <t>坟墓</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否特殊职业</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1369,7 +1369,7 @@
     <tableColumn id="7" name="初始装备" dataDxfId="0"/>
     <tableColumn id="12" name="形象"/>
     <tableColumn id="3" name="颜色"/>
-    <tableColumn id="8" name="是否常规职业"/>
+    <tableColumn id="8" name="是否特殊职业"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1665,7 +1665,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1713,7 +1713,7 @@
         <v>67</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>69</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1789,12 +1789,12 @@
         <v>68</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -1806,7 +1806,7 @@
         <v>94</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1815,7 +1815,7 @@
         <v>72</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1835,7 +1835,7 @@
         <v>95</v>
       </c>
       <c r="F5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>104</v>
@@ -1869,7 +1869,7 @@
         <v>96</v>
       </c>
       <c r="F6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>105</v>
@@ -1901,7 +1901,7 @@
         <v>97</v>
       </c>
       <c r="F7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>107</v>
@@ -1935,7 +1935,7 @@
         <v>98</v>
       </c>
       <c r="F8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>108</v>
@@ -1969,7 +1969,7 @@
         <v>99</v>
       </c>
       <c r="F9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>109</v>
@@ -1982,7 +1982,9 @@
       <c r="K9" t="s">
         <v>85</v>
       </c>
-      <c r="L9" s="7"/>
+      <c r="L9" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2001,7 +2003,7 @@
         <v>100</v>
       </c>
       <c r="F10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>110</v>
@@ -2033,7 +2035,7 @@
         <v>101</v>
       </c>
       <c r="F11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>111</v>
@@ -2065,7 +2067,7 @@
         <v>97</v>
       </c>
       <c r="F12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>113</v>
@@ -2099,7 +2101,7 @@
         <v>102</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>112</v>
@@ -2114,7 +2116,9 @@
       <c r="K13" t="s">
         <v>79</v>
       </c>
-      <c r="L13" s="7"/>
+      <c r="L13" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -2133,7 +2137,7 @@
         <v>103</v>
       </c>
       <c r="F14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>114</v>
@@ -2146,23 +2150,25 @@
       <c r="K14" t="s">
         <v>83</v>
       </c>
-      <c r="L14" s="7"/>
+      <c r="L14" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11001001</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -2174,7 +2180,7 @@
         <v>72</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2182,16 +2188,16 @@
         <v>11001002</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -2203,7 +2209,7 @@
         <v>72</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2358,7 +2364,7 @@
         <v>77</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
balance the job the monster attr
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="143">
   <si>
     <t>arrow</t>
   </si>
@@ -425,10 +425,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>5;5;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>9;10;7</t>
   </si>
   <si>
@@ -598,6 +594,22 @@
   </si>
   <si>
     <t>EnergyRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>8;6;6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>野怪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>10;4;4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>70;15;15</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1351,8 +1363,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L16" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:L16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L17" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:L17"/>
   <tableColumns count="12">
     <tableColumn id="1" name="序列"/>
     <tableColumn id="2" name="名字"/>
@@ -1658,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1709,7 +1721,7 @@
         <v>67</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -1747,7 +1759,7 @@
         <v>69</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
@@ -1767,7 +1779,7 @@
         <v>91</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>36</v>
@@ -1785,12 +1797,12 @@
         <v>68</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -1799,10 +1811,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1811,7 +1823,7 @@
         <v>72</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
@@ -1828,17 +1840,17 @@
         <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1862,13 +1874,13 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -1894,16 +1906,16 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7">
@@ -1928,17 +1940,17 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J8">
         <v>4</v>
@@ -1962,13 +1974,13 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -1979,7 +1991,7 @@
         <v>85</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
@@ -1996,13 +2008,13 @@
         <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -2028,13 +2040,13 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -2060,16 +2072,16 @@
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12">
@@ -2094,16 +2106,16 @@
         <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13">
@@ -2113,7 +2125,7 @@
         <v>79</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
@@ -2130,13 +2142,13 @@
         <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -2147,7 +2159,7 @@
         <v>83</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
@@ -2155,16 +2167,16 @@
         <v>11001001</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -2176,7 +2188,7 @@
         <v>72</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
@@ -2184,16 +2196,16 @@
         <v>11001002</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -2205,7 +2217,36 @@
         <v>72</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>11001003</v>
+      </c>
+      <c r="B17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>72</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2360,7 +2401,7 @@
         <v>77</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
split the job and equip . equip add dura and expire attr
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="148">
   <si>
     <t>arrow</t>
   </si>
@@ -515,10 +515,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>isSpecial</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>true</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -610,6 +606,30 @@
   </si>
   <si>
     <t>70;15;15</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要解锁</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>InitialLocked</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsSpecial</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1260,7 +1280,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1292,6 +1312,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1339,7 +1362,10 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1351,6 +1377,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1363,21 +1457,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L17" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:L17"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:N17" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:N17"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="序列"/>
     <tableColumn id="2" name="名字"/>
     <tableColumn id="19" name="箭矢"/>
     <tableColumn id="33" name="描述"/>
     <tableColumn id="5" name="能量值上限"/>
     <tableColumn id="35" name="魔法点获取的比率"/>
+    <tableColumn id="9" name="技能"/>
     <tableColumn id="4" name="初始的额外卡牌"/>
-    <tableColumn id="6" name="初始道具" dataDxfId="1"/>
-    <tableColumn id="7" name="初始装备" dataDxfId="0"/>
+    <tableColumn id="6" name="初始道具" dataDxfId="2"/>
+    <tableColumn id="7" name="初始装备" dataDxfId="1"/>
     <tableColumn id="12" name="形象"/>
     <tableColumn id="3" name="颜色"/>
     <tableColumn id="8" name="是否特殊职业"/>
+    <tableColumn id="10" name="需要解锁" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1391,7 +1487,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACD"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1670,10 +1766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1683,10 +1779,10 @@
     <col min="4" max="4" width="42.625" customWidth="1"/>
     <col min="5" max="5" width="10.125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="22.25" customWidth="1"/>
+    <col min="7" max="7" width="9.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1706,25 +1802,31 @@
         <v>29</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1744,25 +1846,31 @@
         <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>38</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="N2" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1779,30 +1887,36 @@
         <v>91</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -1811,22 +1925,25 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F4" t="s">
-        <v>127</v>
-      </c>
-      <c r="J4">
+        <v>126</v>
+      </c>
+      <c r="K4">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>72</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M4" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>11000001</v>
       </c>
@@ -1843,24 +1960,28 @@
         <v>93</v>
       </c>
       <c r="F5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5">
+        <v>31000001</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="7"/>
+      <c r="J5" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>1</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>73</v>
       </c>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>11000002</v>
       </c>
@@ -1877,22 +1998,28 @@
         <v>94</v>
       </c>
       <c r="F6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6">
+        <v>31000002</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6">
+      <c r="J6" s="7"/>
+      <c r="K6">
         <v>2</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>74</v>
       </c>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M6" s="7"/>
+      <c r="N6" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>11000003</v>
       </c>
@@ -1909,24 +2036,30 @@
         <v>95</v>
       </c>
       <c r="F7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G7" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G7">
+        <v>31000003</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7">
+      <c r="J7" s="7"/>
+      <c r="K7">
         <v>3</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>75</v>
       </c>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M7" s="7"/>
+      <c r="N7" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>11000004</v>
       </c>
@@ -1943,24 +2076,28 @@
         <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G8" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8">
+        <v>31000004</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="7"/>
+      <c r="J8" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>4</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>76</v>
       </c>
-      <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>11000005</v>
       </c>
@@ -1977,24 +2114,30 @@
         <v>97</v>
       </c>
       <c r="F9" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9">
+        <v>31000005</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9">
+      <c r="J9" s="7"/>
+      <c r="K9">
         <v>5</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>85</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M9" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>11000006</v>
       </c>
@@ -2011,22 +2154,26 @@
         <v>98</v>
       </c>
       <c r="F10" t="s">
-        <v>131</v>
-      </c>
-      <c r="G10" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10">
+        <v>31000006</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10">
+      <c r="J10" s="7"/>
+      <c r="K10">
         <v>6</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>82</v>
       </c>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>11000007</v>
       </c>
@@ -2043,22 +2190,28 @@
         <v>99</v>
       </c>
       <c r="F11" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11">
+        <v>31000007</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11">
+      <c r="J11" s="7"/>
+      <c r="K11">
         <v>7</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>70</v>
       </c>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M11" s="7"/>
+      <c r="N11" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11000008</v>
       </c>
@@ -2075,24 +2228,30 @@
         <v>95</v>
       </c>
       <c r="F12" t="s">
-        <v>133</v>
-      </c>
-      <c r="G12" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G12">
+        <v>31000008</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="I12" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12">
+      <c r="J12" s="7"/>
+      <c r="K12">
         <v>8</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>71</v>
       </c>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M12" s="7"/>
+      <c r="N12" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>11000009</v>
       </c>
@@ -2109,26 +2268,32 @@
         <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>134</v>
-      </c>
-      <c r="G13" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13">
+        <v>31000009</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I13" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13">
+      <c r="J13" s="7"/>
+      <c r="K13">
         <v>9</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>79</v>
       </c>
-      <c r="L13" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M13" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11000010</v>
       </c>
@@ -2145,108 +2310,124 @@
         <v>101</v>
       </c>
       <c r="F14" t="s">
-        <v>135</v>
-      </c>
-      <c r="G14" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14">
+        <v>31000010</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14">
+      <c r="J14" s="7"/>
+      <c r="K14">
         <v>10</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>83</v>
       </c>
-      <c r="L14" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M14" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>11001001</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G15" s="7"/>
+        <v>119</v>
+      </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-      <c r="J15">
+      <c r="J15" s="7"/>
+      <c r="K15">
         <v>0</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>72</v>
       </c>
-      <c r="L15" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M15" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>11001002</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G16" s="7"/>
+        <v>123</v>
+      </c>
+      <c r="G16" s="11"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="J16">
+      <c r="J16" s="7"/>
+      <c r="K16">
         <v>0</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>72</v>
       </c>
-      <c r="L16" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M16" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>11001003</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="E17" t="s">
+        <v>140</v>
+      </c>
+      <c r="F17" t="s">
         <v>141</v>
       </c>
-      <c r="F17" t="s">
-        <v>142</v>
-      </c>
-      <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17">
+      <c r="J17" s="7"/>
+      <c r="K17">
         <v>0</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>72</v>
       </c>
-      <c r="L17" s="7" t="s">
-        <v>119</v>
+      <c r="M17" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2401,7 +2582,7 @@
         <v>77</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add a discover spell card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="148">
   <si>
     <t>arrow</t>
   </si>
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1406,62 +1406,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1845,76 +1789,64 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1927,37 +1859,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:N17" totalsRowShown="0" headerRowDxfId="0" dataDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:N17" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="A3:N17"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="Id" dataDxfId="16"/>
-    <tableColumn id="2" name="Name" dataDxfId="15"/>
-    <tableColumn id="3" name="Arrow" dataDxfId="14"/>
-    <tableColumn id="4" name="Des" dataDxfId="13"/>
-    <tableColumn id="5" name="EnergyLimit" dataDxfId="12"/>
-    <tableColumn id="6" name="EnergyRate" dataDxfId="11"/>
-    <tableColumn id="7" name="SkillId" dataDxfId="10"/>
-    <tableColumn id="8" name="InitialCards" dataDxfId="9"/>
-    <tableColumn id="9" name="InitialItem" dataDxfId="8"/>
-    <tableColumn id="10" name="InitialEquip" dataDxfId="7"/>
-    <tableColumn id="11" name="JobIndex" dataDxfId="6"/>
-    <tableColumn id="12" name="Color" dataDxfId="5"/>
-    <tableColumn id="13" name="IsSpecial" dataDxfId="4"/>
-    <tableColumn id="14" name="InitialLocked" dataDxfId="3"/>
+    <tableColumn id="1" name="Id" dataDxfId="13"/>
+    <tableColumn id="2" name="Name" dataDxfId="12"/>
+    <tableColumn id="3" name="Arrow" dataDxfId="11"/>
+    <tableColumn id="4" name="Des" dataDxfId="10"/>
+    <tableColumn id="5" name="EnergyLimit" dataDxfId="9"/>
+    <tableColumn id="6" name="EnergyRate" dataDxfId="8"/>
+    <tableColumn id="7" name="SkillId" dataDxfId="7"/>
+    <tableColumn id="8" name="InitialCards" dataDxfId="6"/>
+    <tableColumn id="9" name="InitialItem" dataDxfId="5"/>
+    <tableColumn id="10" name="InitialEquip" dataDxfId="4"/>
+    <tableColumn id="11" name="JobIndex" dataDxfId="3"/>
+    <tableColumn id="12" name="Color" dataDxfId="2"/>
+    <tableColumn id="13" name="IsSpecial" dataDxfId="1"/>
+    <tableColumn id="14" name="InitialLocked" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2025,6 +1957,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2060,6 +2009,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2239,7 +2205,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2253,7 +2219,7 @@
     <col min="8" max="8" width="16.25" customWidth="1"/>
     <col min="9" max="9" width="15.125" customWidth="1"/>
     <col min="10" max="10" width="16.25" customWidth="1"/>
-    <col min="11" max="11" width="11.75" customWidth="1"/>
+    <col min="11" max="11" width="6.875" customWidth="1"/>
     <col min="13" max="13" width="12.875" customWidth="1"/>
     <col min="14" max="14" width="17.375" customWidth="1"/>
   </cols>
@@ -2611,9 +2577,7 @@
       <c r="L9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="M9" s="11" t="s">
-        <v>118</v>
-      </c>
+      <c r="M9" s="11"/>
       <c r="N9" s="11" t="s">
         <v>118</v>
       </c>
@@ -2767,9 +2731,7 @@
       <c r="L13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="M13" s="11" t="s">
-        <v>118</v>
-      </c>
+      <c r="M13" s="11"/>
       <c r="N13" s="11" t="s">
         <v>118</v>
       </c>
@@ -2807,9 +2769,7 @@
       <c r="L14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="M14" s="11" t="s">
-        <v>118</v>
-      </c>
+      <c r="M14" s="11"/>
       <c r="N14" s="11" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
auto open job when level up
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Job.xlsx
+++ b/ConfigData/Xlsx/Job.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="146">
   <si>
     <t>arrow</t>
   </si>
@@ -586,10 +586,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>InitialLocked</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>IsSpecial</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -622,6 +618,10 @@
   </si>
   <si>
     <t>51000186,52000020</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LevelNeed</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1306,7 +1306,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1350,6 +1350,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1897,7 +1900,7 @@
     <tableColumn id="11" name="JobIndex" dataDxfId="3"/>
     <tableColumn id="12" name="Color" dataDxfId="2"/>
     <tableColumn id="13" name="IsSpecial" dataDxfId="1"/>
-    <tableColumn id="14" name="InitialLocked" dataDxfId="0"/>
+    <tableColumn id="14" name="LevelNeed" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2227,7 +2230,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2243,7 +2246,7 @@
     <col min="11" max="11" width="8.125" customWidth="1"/>
     <col min="12" max="12" width="6.875" customWidth="1"/>
     <col min="14" max="14" width="5.375" customWidth="1"/>
-    <col min="15" max="15" width="5.625" customWidth="1"/>
+    <col min="15" max="15" width="6.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2251,7 +2254,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>20</v>
@@ -2298,7 +2301,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>18</v>
@@ -2322,10 +2325,10 @@
         <v>35</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>65</v>
@@ -2337,7 +2340,7 @@
         <v>108</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
@@ -2345,7 +2348,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>14</v>
@@ -2381,10 +2384,10 @@
         <v>67</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
@@ -2392,7 +2395,7 @@
         <v>11000000</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
@@ -2420,9 +2423,7 @@
       <c r="N4" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="O4" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="O4" s="15"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
@@ -2448,7 +2449,7 @@
         <v>31000001</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -2496,8 +2497,8 @@
         <v>73</v>
       </c>
       <c r="N6" s="11"/>
-      <c r="O6" s="11" t="s">
-        <v>109</v>
+      <c r="O6" s="15">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
@@ -2535,8 +2536,8 @@
         <v>74</v>
       </c>
       <c r="N7" s="11"/>
-      <c r="O7" s="11" t="s">
-        <v>109</v>
+      <c r="O7" s="15">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
@@ -2563,7 +2564,7 @@
         <v>31000004</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -2611,8 +2612,8 @@
         <v>84</v>
       </c>
       <c r="N9" s="11"/>
-      <c r="O9" s="11" t="s">
-        <v>109</v>
+      <c r="O9" s="15">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
@@ -2639,7 +2640,7 @@
         <v>31000006</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
@@ -2687,8 +2688,8 @@
         <v>69</v>
       </c>
       <c r="N11" s="11"/>
-      <c r="O11" s="11" t="s">
-        <v>109</v>
+      <c r="O11" s="15">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
@@ -2726,8 +2727,8 @@
         <v>70</v>
       </c>
       <c r="N12" s="11"/>
-      <c r="O12" s="11" t="s">
-        <v>109</v>
+      <c r="O12" s="15">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.15">
@@ -2765,8 +2766,8 @@
         <v>78</v>
       </c>
       <c r="N13" s="11"/>
-      <c r="O13" s="11" t="s">
-        <v>109</v>
+      <c r="O13" s="15">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
@@ -2804,8 +2805,8 @@
         <v>82</v>
       </c>
       <c r="N14" s="11"/>
-      <c r="O14" s="11" t="s">
-        <v>109</v>
+      <c r="O14" s="15">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
@@ -2839,9 +2840,7 @@
       <c r="N15" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="O15" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="O15" s="15"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
@@ -2874,9 +2873,7 @@
       <c r="N16" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="O16" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="O16" s="15"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
@@ -2909,9 +2906,7 @@
       <c r="N17" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="O17" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="O17" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>